<commit_message>
- ajout liste d'expression et de mots par émotions - algorithme pour la detection des mots et expressions dans un texte, puis de le catégoriser dans une émotion - status 1 - modification de l'emploi du temps
</commit_message>
<xml_diff>
--- a/projet final/emploi du temps.xlsx
+++ b/projet final/emploi du temps.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Desktop\projet ML\project-Romain\projet final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="270" yWindow="600" windowWidth="17415" windowHeight="8385"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>Emploi du temps</t>
   </si>
@@ -74,16 +79,19 @@
   </si>
   <si>
     <t>analyse, recherche et test de différents algorithmes ML + rendu du status 1</t>
+  </si>
+  <si>
+    <t>analyse, recherche et test de différents algorithmes ML + recherche liste de mots en anglais par émotions + recherche d'api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd&quot; &quot;d&quot; &quot;mmmm&quot; &quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -154,6 +162,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -200,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,9 +248,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,6 +283,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -441,25 +459,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42755</v>
       </c>
@@ -467,19 +485,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42756</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42757</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42758</v>
       </c>
@@ -487,7 +505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42759</v>
       </c>
@@ -495,7 +513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42760</v>
       </c>
@@ -503,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42761</v>
       </c>
@@ -511,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42762</v>
       </c>
@@ -519,7 +537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42763</v>
       </c>
@@ -527,7 +545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>42764</v>
       </c>
@@ -535,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42765</v>
       </c>
@@ -543,47 +561,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42766</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>42767</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>42768</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>42769</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>42770</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>42771</v>
       </c>
@@ -591,7 +609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>42772</v>
       </c>
@@ -599,7 +617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>42773</v>
       </c>
@@ -607,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>42774</v>
       </c>
@@ -615,7 +633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42775</v>
       </c>
@@ -623,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42776</v>
       </c>
@@ -631,7 +649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42777</v>
       </c>
@@ -639,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42778</v>
       </c>
@@ -647,7 +665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>42779</v>
       </c>
@@ -655,7 +673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>42780</v>
       </c>
@@ -663,7 +681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>42781</v>
       </c>
@@ -671,7 +689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>42782</v>
       </c>
@@ -679,7 +697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>42783</v>
       </c>
@@ -687,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>42784</v>
       </c>
@@ -695,7 +713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>42785</v>
       </c>
@@ -703,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>42786</v>
       </c>
@@ -711,7 +729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>42787</v>
       </c>
@@ -719,7 +737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>42788</v>
       </c>
@@ -727,7 +745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>42789</v>
       </c>
@@ -735,7 +753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>42790</v>
       </c>
@@ -743,7 +761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>42791</v>
       </c>
@@ -751,7 +769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1">
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>42792</v>
       </c>
@@ -759,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1">
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>42793</v>
       </c>
@@ -767,7 +785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>42794</v>
       </c>
@@ -775,7 +793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42795</v>
       </c>
@@ -783,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>42796</v>
       </c>
@@ -791,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>42797</v>
       </c>
@@ -799,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1">
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>42798</v>
       </c>
@@ -807,7 +825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1">
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>42799</v>
       </c>
@@ -815,7 +833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1">
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>42800</v>
       </c>
@@ -823,7 +841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1">
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>42801</v>
       </c>
@@ -831,7 +849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1">
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>42802</v>
       </c>
@@ -839,7 +857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1">
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>42803</v>
       </c>
@@ -847,7 +865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1">
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>42804</v>
       </c>
@@ -855,7 +873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1">
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>42805</v>
       </c>
@@ -863,7 +881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1">
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>42806</v>
       </c>
@@ -871,7 +889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>42807</v>
       </c>
@@ -879,7 +897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1">
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>42808</v>
       </c>
@@ -887,7 +905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1">
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>42809</v>
       </c>
@@ -895,7 +913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1">
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>42810</v>
       </c>

</xml_diff>